<commit_message>
done with basic tests, 1st round
</commit_message>
<xml_diff>
--- a/M2basicTest.xlsx
+++ b/M2basicTest.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bxin/wavefront/activeoptics/matlab/m2/test2003/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D88A0B-25FC-3F42-854F-FBED0D3401A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3000" yWindow="-19600" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -79,15 +88,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -97,39 +110,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -319,25 +337,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="16.71"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -351,7 +374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -386,7 +409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -394,16 +417,16 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>-0.8311</v>
+        <v>-0.83109999999999995</v>
       </c>
       <c r="E3" s="2">
-        <v>-41624.0</v>
+        <v>-41624</v>
       </c>
       <c r="F3" s="2">
-        <v>-340834.0</v>
+        <v>-340834</v>
       </c>
       <c r="G3" s="2">
         <v>192.2</v>
@@ -421,16 +444,16 @@
         <v>-831.1</v>
       </c>
       <c r="L3" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M3" s="2">
         <v>187.31</v>
       </c>
       <c r="N3" s="1">
-        <v>2227.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
@@ -438,22 +461,22 @@
         <v>0.01</v>
       </c>
       <c r="D4" s="2">
-        <v>-0.821</v>
+        <v>-0.82099999999999995</v>
       </c>
       <c r="E4" s="2">
-        <v>-41119.0</v>
+        <v>-41119</v>
       </c>
       <c r="F4" s="2">
-        <v>-336704.0</v>
+        <v>-336704</v>
       </c>
       <c r="G4" s="2">
         <v>192.2</v>
       </c>
       <c r="H4" s="2">
-        <v>159.92</v>
+        <v>159.91999999999999</v>
       </c>
       <c r="I4" s="2">
-        <v>4.77</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="J4" s="2">
         <v>27.6</v>
@@ -462,27 +485,27 @@
         <v>-821.05</v>
       </c>
       <c r="L4" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M4" s="2">
         <v>159.84</v>
       </c>
       <c r="N4" s="2">
-        <v>2229.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="2">
         <v>0.02</v>
       </c>
       <c r="D5" s="2">
-        <v>-0.8111</v>
+        <v>-0.81110000000000004</v>
       </c>
       <c r="E5" s="2">
-        <v>-40618.0</v>
+        <v>-40618</v>
       </c>
       <c r="F5" s="2">
-        <v>-332605.0</v>
+        <v>-332605</v>
       </c>
       <c r="G5" s="2">
         <v>192.2</v>
@@ -491,7 +514,7 @@
         <v>133.1</v>
       </c>
       <c r="I5" s="2">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J5" s="2">
         <v>54.6</v>
@@ -500,27 +523,27 @@
         <v>-811.05</v>
       </c>
       <c r="L5" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M5" s="2">
         <v>133.03</v>
       </c>
       <c r="N5" s="2">
-        <v>2233.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="1">
         <v>0.03</v>
       </c>
       <c r="D6" s="2">
-        <v>-0.801</v>
+        <v>-0.80100000000000005</v>
       </c>
       <c r="E6" s="2">
-        <v>-40115.0</v>
+        <v>-40115</v>
       </c>
       <c r="F6" s="2">
-        <v>-328486.0</v>
+        <v>-328486</v>
       </c>
       <c r="G6" s="2">
         <v>192.2</v>
@@ -532,33 +555,33 @@
         <v>4.2</v>
       </c>
       <c r="J6" s="2">
-        <v>81.9</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="K6" s="2">
         <v>-801.01</v>
       </c>
       <c r="L6" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M6" s="2">
         <v>105.91</v>
       </c>
       <c r="N6" s="2">
-        <v>2234.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="1">
         <v>0.04</v>
       </c>
       <c r="D7" s="2">
-        <v>-0.791</v>
+        <v>-0.79100000000000004</v>
       </c>
       <c r="E7" s="2">
-        <v>-39614.0</v>
+        <v>-39614</v>
       </c>
       <c r="F7" s="2">
-        <v>-324380.0</v>
+        <v>-324380</v>
       </c>
       <c r="G7" s="2">
         <v>192.21</v>
@@ -567,36 +590,36 @@
         <v>78.67</v>
       </c>
       <c r="I7" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J7" s="2">
         <v>109.5</v>
       </c>
       <c r="K7" s="2">
-        <v>-791.0</v>
+        <v>-791</v>
       </c>
       <c r="L7" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M7" s="2">
         <v>78.64</v>
       </c>
       <c r="N7" s="2">
-        <v>2235.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C8" s="1">
         <v>0.05</v>
       </c>
       <c r="D8" s="2">
-        <v>-0.781</v>
+        <v>-0.78100000000000003</v>
       </c>
       <c r="E8" s="2">
-        <v>-39112.0</v>
+        <v>-39112</v>
       </c>
       <c r="F8" s="2">
-        <v>-320271.0</v>
+        <v>-320271</v>
       </c>
       <c r="G8" s="2">
         <v>192.21</v>
@@ -608,36 +631,36 @@
         <v>3.75</v>
       </c>
       <c r="J8" s="2">
-        <v>137.7</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="K8" s="2">
         <v>-780.98</v>
       </c>
       <c r="L8" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M8" s="2">
         <v>50.73</v>
       </c>
       <c r="N8" s="2">
-        <v>2237.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>-0.8301</v>
+        <v>-0.83009999999999995</v>
       </c>
       <c r="E9" s="2">
-        <v>-41571.0</v>
+        <v>-41571</v>
       </c>
       <c r="F9" s="2">
-        <v>-340409.0</v>
+        <v>-340409</v>
       </c>
       <c r="G9" s="2">
         <v>192.21</v>
@@ -655,33 +678,33 @@
         <v>-830.08</v>
       </c>
       <c r="L9" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M9" s="2">
         <v>187.21</v>
       </c>
       <c r="N9" s="2">
-        <v>2241.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C10" s="1">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="D10" s="2">
-        <v>-0.8201</v>
+        <v>-0.82010000000000005</v>
       </c>
       <c r="E10" s="1">
-        <v>-41071.0</v>
+        <v>-41071</v>
       </c>
       <c r="F10" s="2">
-        <v>-336310.0</v>
+        <v>-336310</v>
       </c>
       <c r="G10" s="2">
         <v>192.21</v>
       </c>
       <c r="H10" s="2">
-        <v>160.05</v>
+        <v>160.05000000000001</v>
       </c>
       <c r="I10" s="2">
         <v>4.55</v>
@@ -693,27 +716,27 @@
         <v>-820.09</v>
       </c>
       <c r="L10" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M10" s="2">
         <v>160.04</v>
       </c>
       <c r="N10" s="2">
-        <v>2243.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C11" s="2">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="D11" s="2">
-        <v>-0.8101</v>
+        <v>-0.81010000000000004</v>
       </c>
       <c r="E11" s="2">
-        <v>-40571.0</v>
+        <v>-40571</v>
       </c>
       <c r="F11" s="2">
-        <v>-332219.0</v>
+        <v>-332219</v>
       </c>
       <c r="G11" s="2">
         <v>192.22</v>
@@ -722,7 +745,7 @@
         <v>132.44</v>
       </c>
       <c r="I11" s="2">
-        <v>4.35</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="J11" s="2">
         <v>55.44</v>
@@ -731,27 +754,27 @@
         <v>-810.11</v>
       </c>
       <c r="L11" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M11" s="2">
         <v>131.51</v>
       </c>
       <c r="N11" s="2">
-        <v>2244.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="2">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="D12" s="2">
-        <v>-0.8001</v>
+        <v>-0.80010000000000003</v>
       </c>
       <c r="E12" s="2">
-        <v>-40070.0</v>
+        <v>-40070</v>
       </c>
       <c r="F12" s="2">
-        <v>-328119.0</v>
+        <v>-328119</v>
       </c>
       <c r="G12" s="2">
         <v>192.22</v>
@@ -769,27 +792,27 @@
         <v>-800.11</v>
       </c>
       <c r="L12" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M12" s="2">
         <v>104.8</v>
       </c>
       <c r="N12" s="2">
-        <v>2245.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C13" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="D13" s="2">
-        <v>-0.7901</v>
+        <v>-0.79010000000000002</v>
       </c>
       <c r="E13" s="2">
-        <v>-39571.0</v>
+        <v>-39571</v>
       </c>
       <c r="F13" s="2">
-        <v>-324027.0</v>
+        <v>-324027</v>
       </c>
       <c r="G13" s="2">
         <v>192.22</v>
@@ -807,16 +830,16 @@
         <v>-790.13</v>
       </c>
       <c r="L13" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M13" s="2">
         <v>76.72</v>
       </c>
       <c r="N13" s="2">
-        <v>2246.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -824,16 +847,16 @@
         <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>-0.8305</v>
+        <v>-0.83050000000000002</v>
       </c>
       <c r="E14" s="2">
-        <v>-41590.0</v>
+        <v>-41590</v>
       </c>
       <c r="F14" s="2">
-        <v>-340580.0</v>
+        <v>-340580</v>
       </c>
       <c r="G14" s="2">
         <v>192.22</v>
@@ -851,30 +874,30 @@
         <v>-830.48</v>
       </c>
       <c r="L14" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M14" s="2">
         <v>187.38</v>
       </c>
       <c r="N14" s="2">
-        <v>2253.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
-        <v>-0.8393</v>
+        <v>-0.83930000000000005</v>
       </c>
       <c r="E15" s="2">
-        <v>-42030.0</v>
+        <v>-42030</v>
       </c>
       <c r="F15" s="2">
-        <v>-344182.0</v>
+        <v>-344182</v>
       </c>
       <c r="G15" s="2">
         <v>212.23</v>
@@ -892,27 +915,27 @@
         <v>-839.26</v>
       </c>
       <c r="L15" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M15" s="2">
         <v>206.33</v>
       </c>
       <c r="N15" s="2">
-        <v>2255.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2">
-        <v>-0.8481</v>
+        <v>-0.84809999999999997</v>
       </c>
       <c r="E16" s="2">
-        <v>-42477.0</v>
+        <v>-42477</v>
       </c>
       <c r="F16" s="2">
-        <v>-347830.0</v>
+        <v>-347830</v>
       </c>
       <c r="G16" s="2">
         <v>232.23</v>
@@ -930,27 +953,27 @@
         <v>-848.13</v>
       </c>
       <c r="L16" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M16" s="2">
         <v>225.3</v>
       </c>
       <c r="N16" s="2">
-        <v>2256.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2">
-        <v>-0.8572</v>
+        <v>-0.85719999999999996</v>
       </c>
       <c r="E17" s="2">
-        <v>-42926.0</v>
+        <v>-42926</v>
       </c>
       <c r="F17" s="2">
-        <v>-351539.0</v>
+        <v>-351539</v>
       </c>
       <c r="G17" s="2">
         <v>252.23</v>
@@ -959,7 +982,7 @@
         <v>244.3</v>
       </c>
       <c r="I17" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="J17" s="2">
         <v>0.15</v>
@@ -968,33 +991,33 @@
         <v>-857.17</v>
       </c>
       <c r="L17" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M17" s="2">
         <v>244.28</v>
       </c>
       <c r="N17" s="2">
-        <v>2257.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C18" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="D18" s="2">
-        <v>-0.8662</v>
+        <v>-0.86619999999999997</v>
       </c>
       <c r="E18" s="2">
-        <v>-43382.0</v>
+        <v>-43382</v>
       </c>
       <c r="F18" s="2">
-        <v>-355237.0</v>
+        <v>-355237</v>
       </c>
       <c r="G18" s="2">
         <v>272.23</v>
       </c>
       <c r="H18" s="2">
-        <v>263.21</v>
+        <v>263.20999999999998</v>
       </c>
       <c r="I18" s="2">
         <v>9.1</v>
@@ -1006,33 +1029,33 @@
         <v>-866.22</v>
       </c>
       <c r="L18" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M18" s="2">
         <v>263.24</v>
       </c>
       <c r="N18" s="2">
-        <v>2258.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C19" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2">
-        <v>-0.8753</v>
+        <v>-0.87529999999999997</v>
       </c>
       <c r="E19" s="2">
-        <v>-43838.0</v>
+        <v>-43838</v>
       </c>
       <c r="F19" s="2">
-        <v>-358994.0</v>
+        <v>-358994</v>
       </c>
       <c r="G19" s="2">
         <v>292.23</v>
       </c>
       <c r="H19" s="2">
-        <v>282.21</v>
+        <v>282.20999999999998</v>
       </c>
       <c r="I19" s="2">
         <v>9.94</v>
@@ -1044,16 +1067,16 @@
         <v>-875.37</v>
       </c>
       <c r="L19" s="2">
-        <v>-316.0</v>
+        <v>-316</v>
       </c>
       <c r="M19" s="2">
         <v>282.19</v>
       </c>
       <c r="N19" s="2">
-        <v>2259.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1067,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1102,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1110,43 +1133,43 @@
         <v>14</v>
       </c>
       <c r="C23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2">
         <v>-0.1389</v>
       </c>
       <c r="E23" s="2">
-        <v>-22795.0</v>
+        <v>-22795</v>
       </c>
       <c r="F23" s="2">
-        <v>-186603.0</v>
+        <v>-186603</v>
       </c>
       <c r="G23" s="2">
         <v>16.11</v>
       </c>
       <c r="H23" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I23" s="2">
-        <v>-20.0</v>
+        <v>-20</v>
       </c>
       <c r="J23" s="2">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="K23" s="2">
-        <v>-138.92</v>
+        <v>-138.91999999999999</v>
       </c>
       <c r="L23" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N23" s="2">
-        <v>2320.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
@@ -1154,78 +1177,78 @@
         <v>0.01</v>
       </c>
       <c r="D24" s="2">
-        <v>-0.1289</v>
+        <v>-0.12889999999999999</v>
       </c>
       <c r="E24" s="2">
-        <v>-21153.0</v>
+        <v>-21153</v>
       </c>
       <c r="F24" s="2">
-        <v>-173162.0</v>
+        <v>-173162</v>
       </c>
       <c r="G24" s="2">
         <v>16.11</v>
       </c>
       <c r="H24" s="2">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="I24" s="2">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="J24" s="2">
-        <v>-202.0</v>
+        <v>-202</v>
       </c>
       <c r="K24" s="2">
-        <v>-128.92</v>
+        <v>-128.91999999999999</v>
       </c>
       <c r="L24" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2">
-        <v>139.58</v>
+        <v>139.58000000000001</v>
       </c>
       <c r="N24" s="2">
-        <v>2327.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C25" s="2">
         <v>0.02</v>
       </c>
       <c r="D25" s="2">
-        <v>-0.1189</v>
+        <v>-0.11890000000000001</v>
       </c>
       <c r="E25" s="2">
-        <v>-19511.0</v>
+        <v>-19511</v>
       </c>
       <c r="F25" s="2">
-        <v>-159720.0</v>
+        <v>-159720</v>
       </c>
       <c r="G25" s="2">
         <v>16.11</v>
       </c>
       <c r="H25" s="2">
-        <v>255.0</v>
+        <v>255</v>
       </c>
       <c r="I25" s="2">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="J25" s="2">
-        <v>-430.0</v>
+        <v>-430</v>
       </c>
       <c r="K25" s="2">
         <v>-118.91</v>
       </c>
       <c r="L25" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M25" s="2">
         <v>254.72</v>
       </c>
       <c r="N25" s="2">
-        <v>2330.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C26" s="2">
         <v>0.03</v>
       </c>
@@ -1233,273 +1256,273 @@
         <v>-0.1089</v>
       </c>
       <c r="E26" s="2">
-        <v>-17869.0</v>
+        <v>-17869</v>
       </c>
       <c r="F26" s="2">
-        <v>-146276.0</v>
+        <v>-146276</v>
       </c>
       <c r="G26" s="2">
         <v>16.11</v>
       </c>
       <c r="H26" s="2">
-        <v>379.0</v>
+        <v>379</v>
       </c>
       <c r="I26" s="2">
-        <v>317.0</v>
+        <v>317</v>
       </c>
       <c r="J26" s="2">
-        <v>-678.0</v>
+        <v>-678</v>
       </c>
       <c r="K26" s="2">
         <v>-108.9</v>
       </c>
       <c r="L26" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M26" s="2">
         <v>379.05</v>
       </c>
       <c r="N26" s="2">
-        <v>2333.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C27" s="2">
         <v>0.04</v>
       </c>
       <c r="D27" s="2">
-        <v>-0.0989</v>
+        <v>-9.8900000000000002E-2</v>
       </c>
       <c r="E27" s="2">
-        <v>-16227.0</v>
+        <v>-16227</v>
       </c>
       <c r="F27" s="2">
-        <v>-132834.0</v>
+        <v>-132834</v>
       </c>
       <c r="G27" s="2">
         <v>16.11</v>
       </c>
       <c r="H27" s="2">
-        <v>506.0</v>
+        <v>506</v>
       </c>
       <c r="I27" s="2">
-        <v>442.0</v>
+        <v>442</v>
       </c>
       <c r="J27" s="2">
-        <v>-932.0</v>
+        <v>-932</v>
       </c>
       <c r="K27" s="2">
         <v>-98.89</v>
       </c>
       <c r="L27" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M27" s="2">
         <v>506.78</v>
       </c>
       <c r="N27" s="2">
-        <v>2335.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C28" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2">
         <v>-0.1389</v>
       </c>
       <c r="E29" s="2">
-        <v>-22795.0</v>
+        <v>-22795</v>
       </c>
       <c r="F29" s="2">
-        <v>-186603.0</v>
+        <v>-186603</v>
       </c>
       <c r="G29" s="2">
         <v>16.11</v>
       </c>
       <c r="H29" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I29" s="2">
-        <v>-20.0</v>
+        <v>-20</v>
       </c>
       <c r="J29" s="2">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="K29" s="2">
-        <v>-138.92</v>
+        <v>-138.91999999999999</v>
       </c>
       <c r="L29" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N29" s="2">
-        <v>2320.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C30" s="2">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="D30" s="2">
-        <v>-0.1354</v>
+        <v>-0.13539999999999999</v>
       </c>
       <c r="E30" s="2">
-        <v>-22214.0</v>
+        <v>-22214</v>
       </c>
       <c r="F30" s="2">
-        <v>-181846.0</v>
+        <v>-181846</v>
       </c>
       <c r="G30" s="2">
         <v>16.11</v>
       </c>
       <c r="H30" s="2">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="I30" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="J30" s="2">
-        <v>-64.0</v>
+        <v>-64</v>
       </c>
       <c r="K30" s="2">
         <v>-135.38</v>
       </c>
       <c r="L30" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M30" s="2">
-        <v>69.9</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="N30" s="2">
-        <v>2339.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C31" s="2">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="D31" s="2">
         <v>-0.1323</v>
       </c>
       <c r="E31" s="2">
-        <v>-21715.0</v>
+        <v>-21715</v>
       </c>
       <c r="F31" s="2">
-        <v>-177759.0</v>
+        <v>-177759</v>
       </c>
       <c r="G31" s="2">
         <v>16.11</v>
       </c>
       <c r="H31" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="I31" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="J31" s="2">
-        <v>-107.0</v>
+        <v>-107</v>
       </c>
       <c r="K31" s="2">
         <v>-132.34</v>
       </c>
       <c r="L31" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M31" s="2">
         <v>91.7</v>
       </c>
       <c r="N31" s="2">
-        <v>2341.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C32" s="2">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="D32" s="2">
         <v>-0.1293</v>
       </c>
       <c r="E32" s="2">
-        <v>-21215.0</v>
+        <v>-21215</v>
       </c>
       <c r="F32" s="2">
-        <v>-173671.0</v>
+        <v>-173671</v>
       </c>
       <c r="G32" s="2">
         <v>16.11</v>
       </c>
       <c r="H32" s="2">
-        <v>123.0</v>
+        <v>123</v>
       </c>
       <c r="I32" s="2">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="J32" s="2">
-        <v>-171.0</v>
+        <v>-171</v>
       </c>
       <c r="K32" s="2">
-        <v>-129.3</v>
+        <v>-129.30000000000001</v>
       </c>
       <c r="L32" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
         <v>123.96</v>
       </c>
       <c r="N32" s="2">
-        <v>2343.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C33" s="2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="D33" s="2">
-        <v>-0.1262</v>
+        <v>-0.12620000000000001</v>
       </c>
       <c r="E33" s="2">
-        <v>-20715.0</v>
+        <v>-20715</v>
       </c>
       <c r="F33" s="2">
-        <v>-1679575.0</v>
+        <v>-169575</v>
       </c>
       <c r="G33" s="2">
         <v>16.11</v>
       </c>
       <c r="H33" s="2">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="I33" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="J33" s="2">
-        <v>-244.0</v>
+        <v>-244</v>
       </c>
       <c r="K33" s="2">
         <v>-126.25</v>
       </c>
       <c r="L33" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M33" s="2">
-        <v>160.7</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="N33" s="2">
-        <v>2345.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
@@ -1507,133 +1530,133 @@
         <v>18</v>
       </c>
       <c r="C34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2">
         <v>-0.1389</v>
       </c>
       <c r="E34" s="2">
-        <v>-22795.0</v>
+        <v>-22795</v>
       </c>
       <c r="F34" s="2">
-        <v>-186603.0</v>
+        <v>-186603</v>
       </c>
       <c r="G34" s="2">
         <v>16.11</v>
       </c>
       <c r="H34" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I34" s="2">
-        <v>-20.0</v>
+        <v>-20</v>
       </c>
       <c r="J34" s="2">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="K34" s="2">
-        <v>-138.92</v>
+        <v>-138.91999999999999</v>
       </c>
       <c r="L34" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N34" s="2">
-        <v>2320.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D35" s="2">
-        <v>-0.1377</v>
+        <v>-0.13769999999999999</v>
       </c>
       <c r="E35" s="2">
-        <v>-22600.0</v>
+        <v>-22600</v>
       </c>
       <c r="F35" s="2">
-        <v>-184870.0</v>
+        <v>-184870</v>
       </c>
       <c r="G35" s="2">
         <v>36.11</v>
       </c>
       <c r="H35" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="I35" s="2">
-        <v>-11.0</v>
+        <v>-11</v>
       </c>
       <c r="J35" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="K35" s="2">
-        <v>-137.67</v>
+        <v>-137.66999999999999</v>
       </c>
       <c r="L35" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M35" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="N35" s="2">
-        <v>2347.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C36" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="D36" s="2">
-        <v>-0.1367</v>
+        <v>-0.13669999999999999</v>
       </c>
       <c r="E36" s="2">
-        <v>-22449.0</v>
+        <v>-22449</v>
       </c>
       <c r="F36" s="2">
-        <v>-183604.0</v>
+        <v>-183604</v>
       </c>
       <c r="G36" s="2">
         <v>56.11</v>
       </c>
       <c r="H36" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="I36" s="2">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="J36" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="2">
         <v>-136.66</v>
       </c>
       <c r="L36" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="N36" s="2">
-        <v>2350.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C37" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D37" s="2">
-        <v>-0.1359</v>
+        <v>-0.13589999999999999</v>
       </c>
       <c r="E37" s="2">
-        <v>-22275.0</v>
+        <v>-22275</v>
       </c>
       <c r="F37" s="2">
-        <v>-182107.0</v>
+        <v>-182107</v>
       </c>
       <c r="G37" s="2">
         <v>76.11</v>
@@ -1648,36 +1671,36 @@
         <v>-1.47</v>
       </c>
       <c r="K37" s="2">
-        <v>-136.0</v>
+        <v>-136</v>
       </c>
       <c r="L37" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M37" s="2">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="N37" s="2">
-        <v>2352.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C38" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="D38" s="2">
         <v>-0.1348</v>
       </c>
       <c r="E38" s="2">
-        <v>-22148.0</v>
+        <v>-22148</v>
       </c>
       <c r="F38" s="2">
-        <v>-181318.0</v>
+        <v>-181318</v>
       </c>
       <c r="G38" s="2">
         <v>96.11</v>
       </c>
       <c r="H38" s="2">
-        <v>77.99</v>
+        <v>77.989999999999995</v>
       </c>
       <c r="I38" s="2">
         <v>17.38</v>
@@ -1689,27 +1712,27 @@
         <v>-134.94</v>
       </c>
       <c r="L38" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="N38" s="2">
-        <v>2356.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C39" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D39" s="2">
-        <v>-0.1339</v>
+        <v>-0.13389999999999999</v>
       </c>
       <c r="E39" s="2">
-        <v>-21973.0</v>
+        <v>-21973</v>
       </c>
       <c r="F39" s="2">
-        <v>-180064.0</v>
+        <v>-180064</v>
       </c>
       <c r="G39" s="1">
         <v>116.11</v>
@@ -1727,19 +1750,18 @@
         <v>-133.94</v>
       </c>
       <c r="L39" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M39" s="2">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="N39" s="2">
-        <v>2357.0</v>
+        <v>2357</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>